<commit_message>
updating analysis and readme
</commit_message>
<xml_diff>
--- a/Data/Cont Ed Nanocamp Survey.xlsx
+++ b/Data/Cont Ed Nanocamp Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saman\Desktop\Research\Nanocamp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C949319-D602-471A-A2C2-29847DA94DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853B3C3E-D366-43CE-9807-A7F7142F96D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -618,10 +618,10 @@
   <dimension ref="A1:AH36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>